<commit_message>
eval for nE_tsp_50 models
</commit_message>
<xml_diff>
--- a/AM2019/am_eval_log_Jan26.xlsx
+++ b/AM2019/am_eval_log_Jan26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,35 +441,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>decode_strategy</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>width</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>rnd_S</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>rnd_C</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>amz_nS</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>amz_S</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>amz_eval</t>
         </is>
@@ -481,27 +486,30 @@
           <t>icml_nE_tsp20_ref</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>20</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>greedy</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>5.67799711227417</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>4.873636722564697</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>3136.23193359375</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>6747.70703125</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -513,27 +521,30 @@
           <t>icml_nE_tsp20_relK5</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>greedy</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>5.204187393188477</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>4.491534233093262</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>3130.527099609375</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>7309.23291015625</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -545,27 +556,30 @@
           <t>icml_nE_tsp20_relK20</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>greedy</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>0</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>5.140490055084229</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>4.420088291168213</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>3085.472900390625</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>7223.6181640625</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -577,27 +591,30 @@
           <t>icml_nE_tsp20_orgK5</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" t="n">
+        <v>20</v>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>greedy</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>0</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>5.115683078765869</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>4.396299362182617</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>3028.08642578125</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>6532.27392578125</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -609,27 +626,30 @@
           <t>icml_nE_tsp20_orgK20</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="n">
+        <v>20</v>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>greedy</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>0</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>4.953151226043701</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>4.227758884429932</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>2993.077392578125</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>6291.3271484375</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -641,27 +661,30 @@
           <t>icml_nE_tsp20_orgK20_onlyD</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" t="n">
+        <v>20</v>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>greedy</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>0</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>4.95285177230835</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>4.231305599212646</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>2994.485107421875</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>6324.755859375</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -673,27 +696,30 @@
           <t>icml_nE_tsp20_relE1</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" t="n">
+        <v>20</v>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>greedy</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>0</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>5.071157455444336</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>4.367247104644775</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>3088.646728515625</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>7663.43603515625</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -705,27 +731,30 @@
           <t>icml_nE_tsp20_relE3</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" t="n">
+        <v>20</v>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>greedy</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>0</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>4.959534168243408</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>4.267938137054443</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>3087.42529296875</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>7574.6689453125</v>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -737,27 +766,30 @@
           <t>icml_nE_tsp20_orgE1</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" t="n">
+        <v>20</v>
+      </c>
+      <c r="C10" t="inlineStr">
         <is>
           <t>greedy</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>0</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>5.031073093414307</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>4.325075626373291</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>3038.4833984375</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>7052.419921875</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -769,27 +801,30 @@
           <t>icml_nE_tsp20_orgE3</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" t="n">
+        <v>20</v>
+      </c>
+      <c r="C11" t="inlineStr">
         <is>
           <t>greedy</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>0</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>4.905350685119629</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>4.206727504730225</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>2997.14111328125</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>6919.68896484375</v>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -801,27 +836,30 @@
           <t>icml_nE_tsp20_relK5_orgE1</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" t="n">
+        <v>20</v>
+      </c>
+      <c r="C12" t="inlineStr">
         <is>
           <t>greedy</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>0</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>4.976040840148926</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>4.27073335647583</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>3037.77783203125</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>7018.42578125</v>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -833,27 +871,30 @@
           <t>icml_nE_tsp20_relK5_orgE3</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" t="n">
+        <v>20</v>
+      </c>
+      <c r="C13" t="inlineStr">
         <is>
           <t>greedy</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>0</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>4.898928642272949</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>4.206792831420898</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>3009.0908203125</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>6866.6494140625</v>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -862,30 +903,33 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_ref</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>1000</v>
+          <t>icml_nE_tsp20_relK5_orgE6_ultra</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>20</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
       </c>
       <c r="D14" t="n">
-        <v>5.484336376190186</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>4.688866138458252</v>
+        <v>4.836507797241211</v>
       </c>
       <c r="F14" t="n">
-        <v>2993.2412109375</v>
+        <v>4.140256881713867</v>
       </c>
       <c r="G14" t="n">
-        <v>6690.89892578125</v>
-      </c>
-      <c r="H14" t="inlineStr">
+        <v>2952.123046875</v>
+      </c>
+      <c r="H14" t="n">
+        <v>6711.28759765625</v>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -894,30 +938,33 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_relK5</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
+          <t>icml_nE_tsp20_ref</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>20</v>
+      </c>
+      <c r="C15" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>1000</v>
-      </c>
       <c r="D15" t="n">
-        <v>5.032746315002441</v>
+        <v>1000</v>
       </c>
       <c r="E15" t="n">
-        <v>4.310319423675537</v>
+        <v>5.484336376190186</v>
       </c>
       <c r="F15" t="n">
-        <v>2981.19677734375</v>
+        <v>4.688866138458252</v>
       </c>
       <c r="G15" t="n">
-        <v>6659.5693359375</v>
-      </c>
-      <c r="H15" t="inlineStr">
+        <v>2993.2412109375</v>
+      </c>
+      <c r="H15" t="n">
+        <v>6690.89892578125</v>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -926,30 +973,33 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_relK20</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
+          <t>icml_nE_tsp20_relK5</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>20</v>
+      </c>
+      <c r="C16" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>1000</v>
-      </c>
       <c r="D16" t="n">
-        <v>4.973409175872803</v>
+        <v>1000</v>
       </c>
       <c r="E16" t="n">
-        <v>4.265445232391357</v>
+        <v>5.032746315002441</v>
       </c>
       <c r="F16" t="n">
-        <v>2955.710693359375</v>
+        <v>4.310319423675537</v>
       </c>
       <c r="G16" t="n">
-        <v>6623.8828125</v>
-      </c>
-      <c r="H16" t="inlineStr">
+        <v>2981.19677734375</v>
+      </c>
+      <c r="H16" t="n">
+        <v>6659.5693359375</v>
+      </c>
+      <c r="I16" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -958,30 +1008,33 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_orgK5</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
+          <t>icml_nE_tsp20_relK20</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>20</v>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="C17" t="n">
-        <v>1000</v>
-      </c>
       <c r="D17" t="n">
-        <v>4.938973903656006</v>
+        <v>1000</v>
       </c>
       <c r="E17" t="n">
-        <v>4.226493358612061</v>
+        <v>4.973409175872803</v>
       </c>
       <c r="F17" t="n">
-        <v>2920.355712890625</v>
+        <v>4.265445232391357</v>
       </c>
       <c r="G17" t="n">
-        <v>6189.6259765625</v>
-      </c>
-      <c r="H17" t="inlineStr">
+        <v>2955.710693359375</v>
+      </c>
+      <c r="H17" t="n">
+        <v>6623.8828125</v>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -990,30 +1043,33 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_orgK20</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
+          <t>icml_nE_tsp20_orgK5</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>20</v>
+      </c>
+      <c r="C18" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="C18" t="n">
-        <v>1000</v>
-      </c>
       <c r="D18" t="n">
-        <v>4.815895557403564</v>
+        <v>1000</v>
       </c>
       <c r="E18" t="n">
-        <v>4.118557453155518</v>
+        <v>4.938973903656006</v>
       </c>
       <c r="F18" t="n">
-        <v>2897.786865234375</v>
+        <v>4.226493358612061</v>
       </c>
       <c r="G18" t="n">
-        <v>6071.34130859375</v>
-      </c>
-      <c r="H18" t="inlineStr">
+        <v>2920.355712890625</v>
+      </c>
+      <c r="H18" t="n">
+        <v>6189.6259765625</v>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1022,30 +1078,33 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_orgK20_onlyD</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
+          <t>icml_nE_tsp20_orgK20</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>20</v>
+      </c>
+      <c r="C19" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="C19" t="n">
-        <v>1000</v>
-      </c>
       <c r="D19" t="n">
-        <v>4.820348262786865</v>
+        <v>1000</v>
       </c>
       <c r="E19" t="n">
-        <v>4.122185707092285</v>
+        <v>4.815895557403564</v>
       </c>
       <c r="F19" t="n">
-        <v>2907.909423828125</v>
+        <v>4.118557453155518</v>
       </c>
       <c r="G19" t="n">
-        <v>6022.42822265625</v>
-      </c>
-      <c r="H19" t="inlineStr">
+        <v>2897.786865234375</v>
+      </c>
+      <c r="H19" t="n">
+        <v>6071.34130859375</v>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1054,30 +1113,33 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_relE1</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
+          <t>icml_nE_tsp20_orgK20_onlyD</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>20</v>
+      </c>
+      <c r="C20" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="C20" t="n">
-        <v>1000</v>
-      </c>
       <c r="D20" t="n">
-        <v>4.905979633331299</v>
+        <v>1000</v>
       </c>
       <c r="E20" t="n">
-        <v>4.20769214630127</v>
+        <v>4.820348262786865</v>
       </c>
       <c r="F20" t="n">
-        <v>2950.119140625</v>
+        <v>4.122185707092285</v>
       </c>
       <c r="G20" t="n">
-        <v>6924.6064453125</v>
-      </c>
-      <c r="H20" t="inlineStr">
+        <v>2907.909423828125</v>
+      </c>
+      <c r="H20" t="n">
+        <v>6022.42822265625</v>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1086,30 +1148,33 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_relE3</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
+          <t>icml_nE_tsp20_relE1</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="C21" t="n">
-        <v>1000</v>
-      </c>
       <c r="D21" t="n">
-        <v>4.82759952545166</v>
+        <v>1000</v>
       </c>
       <c r="E21" t="n">
-        <v>4.138593673706055</v>
+        <v>4.905979633331299</v>
       </c>
       <c r="F21" t="n">
-        <v>2932.60888671875</v>
+        <v>4.20769214630127</v>
       </c>
       <c r="G21" t="n">
-        <v>6911.31298828125</v>
-      </c>
-      <c r="H21" t="inlineStr">
+        <v>2950.119140625</v>
+      </c>
+      <c r="H21" t="n">
+        <v>6924.6064453125</v>
+      </c>
+      <c r="I21" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1118,30 +1183,33 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_orgE1</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
+          <t>icml_nE_tsp20_relE3</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>20</v>
+      </c>
+      <c r="C22" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="C22" t="n">
-        <v>1000</v>
-      </c>
       <c r="D22" t="n">
-        <v>4.870941638946533</v>
+        <v>1000</v>
       </c>
       <c r="E22" t="n">
-        <v>4.17216157913208</v>
+        <v>4.82759952545166</v>
       </c>
       <c r="F22" t="n">
-        <v>2918.220947265625</v>
+        <v>4.138593673706055</v>
       </c>
       <c r="G22" t="n">
-        <v>6628.1630859375</v>
-      </c>
-      <c r="H22" t="inlineStr">
+        <v>2932.60888671875</v>
+      </c>
+      <c r="H22" t="n">
+        <v>6911.31298828125</v>
+      </c>
+      <c r="I22" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1150,30 +1218,33 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_orgE3</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
+          <t>icml_nE_tsp20_orgE1</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>20</v>
+      </c>
+      <c r="C23" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="C23" t="n">
-        <v>1000</v>
-      </c>
       <c r="D23" t="n">
-        <v>4.796833038330078</v>
+        <v>1000</v>
       </c>
       <c r="E23" t="n">
-        <v>4.110092163085938</v>
+        <v>4.870941638946533</v>
       </c>
       <c r="F23" t="n">
-        <v>2891.521728515625</v>
+        <v>4.17216157913208</v>
       </c>
       <c r="G23" t="n">
-        <v>6581.3349609375</v>
-      </c>
-      <c r="H23" t="inlineStr">
+        <v>2918.220947265625</v>
+      </c>
+      <c r="H23" t="n">
+        <v>6628.1630859375</v>
+      </c>
+      <c r="I23" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1182,30 +1253,33 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_relK5_orgE1</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
+          <t>icml_nE_tsp20_orgE3</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>20</v>
+      </c>
+      <c r="C24" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="C24" t="n">
-        <v>1000</v>
-      </c>
       <c r="D24" t="n">
-        <v>4.848568916320801</v>
+        <v>1000</v>
       </c>
       <c r="E24" t="n">
-        <v>4.149362564086914</v>
+        <v>4.796833038330078</v>
       </c>
       <c r="F24" t="n">
-        <v>2919.861572265625</v>
+        <v>4.110092163085938</v>
       </c>
       <c r="G24" t="n">
-        <v>6460.88427734375</v>
-      </c>
-      <c r="H24" t="inlineStr">
+        <v>2891.521728515625</v>
+      </c>
+      <c r="H24" t="n">
+        <v>6581.3349609375</v>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1214,30 +1288,33 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_relK5_orgE3</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
+          <t>icml_nE_tsp20_relK5_orgE1</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>20</v>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="C25" t="n">
-        <v>1000</v>
-      </c>
       <c r="D25" t="n">
-        <v>4.801133632659912</v>
+        <v>1000</v>
       </c>
       <c r="E25" t="n">
-        <v>4.109539031982422</v>
+        <v>4.848568916320801</v>
       </c>
       <c r="F25" t="n">
-        <v>2897.54638671875</v>
+        <v>4.149362564086914</v>
       </c>
       <c r="G25" t="n">
-        <v>6394.10107421875</v>
-      </c>
-      <c r="H25" t="inlineStr">
+        <v>2919.861572265625</v>
+      </c>
+      <c r="H25" t="n">
+        <v>6460.88427734375</v>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1246,30 +1323,33 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_ref</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>bs</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>1000</v>
+          <t>icml_nE_tsp20_relK5_orgE3</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>20</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
       </c>
       <c r="D26" t="n">
-        <v>5.206974506378174</v>
+        <v>1000</v>
       </c>
       <c r="E26" t="n">
-        <v>4.479283332824707</v>
+        <v>4.801133632659912</v>
       </c>
       <c r="F26" t="n">
-        <v>2934.550048828125</v>
+        <v>4.109539031982422</v>
       </c>
       <c r="G26" t="n">
-        <v>6386.1611328125</v>
-      </c>
-      <c r="H26" t="inlineStr">
+        <v>2897.54638671875</v>
+      </c>
+      <c r="H26" t="n">
+        <v>6394.10107421875</v>
+      </c>
+      <c r="I26" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1278,30 +1358,33 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_relK5</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>bs</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>1000</v>
+          <t>icml_nE_tsp20_relK5_orgE6_ultra</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>20</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
       </c>
       <c r="D27" t="n">
-        <v>4.878531455993652</v>
+        <v>1000</v>
       </c>
       <c r="E27" t="n">
-        <v>4.203481674194336</v>
+        <v>4.740680694580078</v>
       </c>
       <c r="F27" t="n">
-        <v>2936.192138671875</v>
+        <v>4.065781116485596</v>
       </c>
       <c r="G27" t="n">
-        <v>6734.61669921875</v>
-      </c>
-      <c r="H27" t="inlineStr">
+        <v>2851.4189453125</v>
+      </c>
+      <c r="H27" t="n">
+        <v>6268.69287109375</v>
+      </c>
+      <c r="I27" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1310,30 +1393,33 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_relK20</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
+          <t>icml_nE_tsp20_ref</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>20</v>
+      </c>
+      <c r="C28" t="inlineStr">
         <is>
           <t>bs</t>
         </is>
       </c>
-      <c r="C28" t="n">
-        <v>1000</v>
-      </c>
       <c r="D28" t="n">
-        <v>4.843759536743164</v>
+        <v>1000</v>
       </c>
       <c r="E28" t="n">
-        <v>4.164356708526611</v>
+        <v>5.206974506378174</v>
       </c>
       <c r="F28" t="n">
-        <v>2903.51953125</v>
+        <v>4.479283332824707</v>
       </c>
       <c r="G28" t="n">
-        <v>6687.33837890625</v>
-      </c>
-      <c r="H28" t="inlineStr">
+        <v>2934.550048828125</v>
+      </c>
+      <c r="H28" t="n">
+        <v>6386.1611328125</v>
+      </c>
+      <c r="I28" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1342,30 +1428,33 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_orgK5</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
+          <t>icml_nE_tsp20_relK5</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>20</v>
+      </c>
+      <c r="C29" t="inlineStr">
         <is>
           <t>bs</t>
         </is>
       </c>
-      <c r="C29" t="n">
-        <v>1000</v>
-      </c>
       <c r="D29" t="n">
-        <v>4.806042194366455</v>
+        <v>1000</v>
       </c>
       <c r="E29" t="n">
-        <v>4.122819423675537</v>
+        <v>4.878531455993652</v>
       </c>
       <c r="F29" t="n">
-        <v>2887.33837890625</v>
+        <v>4.203481674194336</v>
       </c>
       <c r="G29" t="n">
-        <v>6208.02197265625</v>
-      </c>
-      <c r="H29" t="inlineStr">
+        <v>2936.192138671875</v>
+      </c>
+      <c r="H29" t="n">
+        <v>6734.61669921875</v>
+      </c>
+      <c r="I29" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1374,30 +1463,33 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_orgK20</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
+          <t>icml_nE_tsp20_relK20</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>20</v>
+      </c>
+      <c r="C30" t="inlineStr">
         <is>
           <t>bs</t>
         </is>
       </c>
-      <c r="C30" t="n">
-        <v>1000</v>
-      </c>
       <c r="D30" t="n">
-        <v>4.73866081237793</v>
+        <v>1000</v>
       </c>
       <c r="E30" t="n">
-        <v>4.065176963806152</v>
+        <v>4.843759536743164</v>
       </c>
       <c r="F30" t="n">
-        <v>2856.151611328125</v>
+        <v>4.164356708526611</v>
       </c>
       <c r="G30" t="n">
-        <v>6034.828125</v>
-      </c>
-      <c r="H30" t="inlineStr">
+        <v>2903.51953125</v>
+      </c>
+      <c r="H30" t="n">
+        <v>6687.33837890625</v>
+      </c>
+      <c r="I30" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1406,30 +1498,33 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_orgK20_onlyD</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
+          <t>icml_nE_tsp20_orgK5</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>20</v>
+      </c>
+      <c r="C31" t="inlineStr">
         <is>
           <t>bs</t>
         </is>
       </c>
-      <c r="C31" t="n">
-        <v>1000</v>
-      </c>
       <c r="D31" t="n">
-        <v>4.743274211883545</v>
+        <v>1000</v>
       </c>
       <c r="E31" t="n">
-        <v>4.066792488098145</v>
+        <v>4.806042194366455</v>
       </c>
       <c r="F31" t="n">
-        <v>2861.528564453125</v>
+        <v>4.122819423675537</v>
       </c>
       <c r="G31" t="n">
-        <v>6021.4443359375</v>
-      </c>
-      <c r="H31" t="inlineStr">
+        <v>2887.33837890625</v>
+      </c>
+      <c r="H31" t="n">
+        <v>6208.02197265625</v>
+      </c>
+      <c r="I31" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1438,30 +1533,33 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_relE1</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
+          <t>icml_nE_tsp20_orgK20</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>20</v>
+      </c>
+      <c r="C32" t="inlineStr">
         <is>
           <t>bs</t>
         </is>
       </c>
-      <c r="C32" t="n">
-        <v>1000</v>
-      </c>
       <c r="D32" t="n">
-        <v>4.790219783782959</v>
+        <v>1000</v>
       </c>
       <c r="E32" t="n">
-        <v>4.119714260101318</v>
+        <v>4.73866081237793</v>
       </c>
       <c r="F32" t="n">
-        <v>2908.402099609375</v>
+        <v>4.065176963806152</v>
       </c>
       <c r="G32" t="n">
-        <v>7048.49169921875</v>
-      </c>
-      <c r="H32" t="inlineStr">
+        <v>2856.151611328125</v>
+      </c>
+      <c r="H32" t="n">
+        <v>6034.828125</v>
+      </c>
+      <c r="I32" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1470,30 +1568,33 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_relE3</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
+          <t>icml_nE_tsp20_orgK20_onlyD</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>20</v>
+      </c>
+      <c r="C33" t="inlineStr">
         <is>
           <t>bs</t>
         </is>
       </c>
-      <c r="C33" t="n">
-        <v>1000</v>
-      </c>
       <c r="D33" t="n">
-        <v>4.746721267700195</v>
+        <v>1000</v>
       </c>
       <c r="E33" t="n">
-        <v>4.082385540008545</v>
+        <v>4.743274211883545</v>
       </c>
       <c r="F33" t="n">
-        <v>2900.21337890625</v>
+        <v>4.066792488098145</v>
       </c>
       <c r="G33" t="n">
-        <v>6968.3115234375</v>
-      </c>
-      <c r="H33" t="inlineStr">
+        <v>2861.528564453125</v>
+      </c>
+      <c r="H33" t="n">
+        <v>6021.4443359375</v>
+      </c>
+      <c r="I33" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1502,30 +1603,33 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_orgE1</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
+          <t>icml_nE_tsp20_relE1</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>20</v>
+      </c>
+      <c r="C34" t="inlineStr">
         <is>
           <t>bs</t>
         </is>
       </c>
-      <c r="C34" t="n">
-        <v>1000</v>
-      </c>
       <c r="D34" t="n">
-        <v>4.768683433532715</v>
+        <v>1000</v>
       </c>
       <c r="E34" t="n">
-        <v>4.096010684967041</v>
+        <v>4.790219783782959</v>
       </c>
       <c r="F34" t="n">
-        <v>2878.761962890625</v>
+        <v>4.119714260101318</v>
       </c>
       <c r="G34" t="n">
-        <v>6590.02587890625</v>
-      </c>
-      <c r="H34" t="inlineStr">
+        <v>2908.402099609375</v>
+      </c>
+      <c r="H34" t="n">
+        <v>7048.49169921875</v>
+      </c>
+      <c r="I34" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1534,30 +1638,33 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_orgE3</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
+          <t>icml_nE_tsp20_relE3</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>20</v>
+      </c>
+      <c r="C35" t="inlineStr">
         <is>
           <t>bs</t>
         </is>
       </c>
-      <c r="C35" t="n">
-        <v>1000</v>
-      </c>
       <c r="D35" t="n">
-        <v>4.733546733856201</v>
+        <v>1000</v>
       </c>
       <c r="E35" t="n">
-        <v>4.068373203277588</v>
+        <v>4.746721267700195</v>
       </c>
       <c r="F35" t="n">
-        <v>2869.01416015625</v>
+        <v>4.082385540008545</v>
       </c>
       <c r="G35" t="n">
-        <v>6499.54345703125</v>
-      </c>
-      <c r="H35" t="inlineStr">
+        <v>2900.21337890625</v>
+      </c>
+      <c r="H35" t="n">
+        <v>6968.3115234375</v>
+      </c>
+      <c r="I35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1566,30 +1673,33 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>icml_nE_tsp20_relK5_orgE1</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
+          <t>icml_nE_tsp20_orgE1</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>20</v>
+      </c>
+      <c r="C36" t="inlineStr">
         <is>
           <t>bs</t>
         </is>
       </c>
-      <c r="C36" t="n">
-        <v>1000</v>
-      </c>
       <c r="D36" t="n">
-        <v>4.750167846679688</v>
+        <v>1000</v>
       </c>
       <c r="E36" t="n">
-        <v>4.077676773071289</v>
+        <v>4.768683433532715</v>
       </c>
       <c r="F36" t="n">
-        <v>2880.722412109375</v>
+        <v>4.096010684967041</v>
       </c>
       <c r="G36" t="n">
-        <v>6545.0732421875</v>
-      </c>
-      <c r="H36" t="inlineStr">
+        <v>2878.761962890625</v>
+      </c>
+      <c r="H36" t="n">
+        <v>6590.02587890625</v>
+      </c>
+      <c r="I36" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1598,30 +1708,1510 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
+          <t>icml_nE_tsp20_orgE3</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>20</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E37" t="n">
+        <v>4.733546733856201</v>
+      </c>
+      <c r="F37" t="n">
+        <v>4.068373203277588</v>
+      </c>
+      <c r="G37" t="n">
+        <v>2869.01416015625</v>
+      </c>
+      <c r="H37" t="n">
+        <v>6499.54345703125</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp20_relK5_orgE1</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>20</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E38" t="n">
+        <v>4.750167846679688</v>
+      </c>
+      <c r="F38" t="n">
+        <v>4.077676773071289</v>
+      </c>
+      <c r="G38" t="n">
+        <v>2880.722412109375</v>
+      </c>
+      <c r="H38" t="n">
+        <v>6545.0732421875</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
           <t>icml_nE_tsp20_relK5_orgE3</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B39" t="n">
+        <v>20</v>
+      </c>
+      <c r="C39" t="inlineStr">
         <is>
           <t>bs</t>
         </is>
       </c>
-      <c r="C37" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D37" t="n">
+      <c r="D39" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E39" t="n">
         <v>4.734110355377197</v>
       </c>
-      <c r="E37" t="n">
+      <c r="F39" t="n">
         <v>4.065284729003906</v>
       </c>
-      <c r="F37" t="n">
+      <c r="G39" t="n">
         <v>2870.630615234375</v>
       </c>
-      <c r="G37" t="n">
+      <c r="H39" t="n">
         <v>6435.4619140625</v>
       </c>
-      <c r="H37" t="inlineStr">
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp20_relK5_orgE6_ultra</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>20</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E40" t="n">
+        <v>4.710590839385986</v>
+      </c>
+      <c r="F40" t="n">
+        <v>4.048228740692139</v>
+      </c>
+      <c r="G40" t="n">
+        <v>2836.913330078125</v>
+      </c>
+      <c r="H40" t="n">
+        <v>6307.01123046875</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_ref</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>50</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>10.39750957489014</v>
+      </c>
+      <c r="F41" t="n">
+        <v>8.904349327087402</v>
+      </c>
+      <c r="G41" t="n">
+        <v>5888.62060546875</v>
+      </c>
+      <c r="H41" t="n">
+        <v>10781.5263671875</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK5</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>50</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>9.859577178955078</v>
+      </c>
+      <c r="F42" t="n">
+        <v>8.427781105041504</v>
+      </c>
+      <c r="G42" t="n">
+        <v>5555.9775390625</v>
+      </c>
+      <c r="H42" t="n">
+        <v>10989.3359375</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK20</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>50</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>9.709867477416992</v>
+      </c>
+      <c r="F43" t="n">
+        <v>8.328015327453613</v>
+      </c>
+      <c r="G43" t="n">
+        <v>5416.99755859375</v>
+      </c>
+      <c r="H43" t="n">
+        <v>11215.634765625</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_orgK5</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>50</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>9.946928024291992</v>
+      </c>
+      <c r="F44" t="n">
+        <v>8.495722770690918</v>
+      </c>
+      <c r="G44" t="n">
+        <v>5280.74658203125</v>
+      </c>
+      <c r="H44" t="n">
+        <v>10053.595703125</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_orgK20</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>50</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>9.232181549072266</v>
+      </c>
+      <c r="F45" t="n">
+        <v>7.875949382781982</v>
+      </c>
+      <c r="G45" t="n">
+        <v>5252.1611328125</v>
+      </c>
+      <c r="H45" t="n">
+        <v>9213.490234375</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relE1</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>50</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>9.47725772857666</v>
+      </c>
+      <c r="F46" t="n">
+        <v>8.19194507598877</v>
+      </c>
+      <c r="G46" t="n">
+        <v>5488.53515625</v>
+      </c>
+      <c r="H46" t="n">
+        <v>11981.83203125</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relE3</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>50</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>9.14936351776123</v>
+      </c>
+      <c r="F47" t="n">
+        <v>7.848254203796387</v>
+      </c>
+      <c r="G47" t="n">
+        <v>5373.9990234375</v>
+      </c>
+      <c r="H47" t="n">
+        <v>12559.841796875</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_orgE1</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>50</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>9.363945007324219</v>
+      </c>
+      <c r="F48" t="n">
+        <v>8.105080604553223</v>
+      </c>
+      <c r="G48" t="n">
+        <v>5437.4033203125</v>
+      </c>
+      <c r="H48" t="n">
+        <v>10523.974609375</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_orgE3</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>50</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>8.96048641204834</v>
+      </c>
+      <c r="F49" t="n">
+        <v>7.670102596282959</v>
+      </c>
+      <c r="G49" t="n">
+        <v>5243.09228515625</v>
+      </c>
+      <c r="H49" t="n">
+        <v>10806.00390625</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK5_orgE1</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>50</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>9.331015586853027</v>
+      </c>
+      <c r="F50" t="n">
+        <v>8.026241302490234</v>
+      </c>
+      <c r="G50" t="n">
+        <v>5358.3828125</v>
+      </c>
+      <c r="H50" t="n">
+        <v>10909.58203125</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK5_orgE3</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>50</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>8.953964233398438</v>
+      </c>
+      <c r="F51" t="n">
+        <v>7.648116111755371</v>
+      </c>
+      <c r="G51" t="n">
+        <v>5292.87744140625</v>
+      </c>
+      <c r="H51" t="n">
+        <v>11247.0859375</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK5_orgE6_ultra</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>50</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>greedy</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>8.72899341583252</v>
+      </c>
+      <c r="F52" t="n">
+        <v>7.451225757598877</v>
+      </c>
+      <c r="G52" t="n">
+        <v>5073.7685546875</v>
+      </c>
+      <c r="H52" t="n">
+        <v>10045.50390625</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_ref</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>50</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E53" t="n">
+        <v>9.880249977111816</v>
+      </c>
+      <c r="F53" t="n">
+        <v>8.395107269287109</v>
+      </c>
+      <c r="G53" t="n">
+        <v>5324.0078125</v>
+      </c>
+      <c r="H53" t="n">
+        <v>12955.9365234375</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK5</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>50</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E54" t="n">
+        <v>9.378718376159668</v>
+      </c>
+      <c r="F54" t="n">
+        <v>7.991859436035156</v>
+      </c>
+      <c r="G54" t="n">
+        <v>5220.35400390625</v>
+      </c>
+      <c r="H54" t="n">
+        <v>11397.7841796875</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK20</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>50</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_orgK5</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>50</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_orgK20</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>50</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relE1</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>50</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relE3</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>50</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_orgE1</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>50</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_orgE3</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>50</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E61" t="n">
+        <v>8.652674674987793</v>
+      </c>
+      <c r="F61" t="n">
+        <v>7.378743171691895</v>
+      </c>
+      <c r="G61" t="n">
+        <v>4971.7578125</v>
+      </c>
+      <c r="H61" t="n">
+        <v>12577.5439453125</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK5_orgE1</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>50</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK5_orgE3</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>50</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E63" t="n">
+        <v>8.662599563598633</v>
+      </c>
+      <c r="F63" t="n">
+        <v>7.375399589538574</v>
+      </c>
+      <c r="G63" t="n">
+        <v>5064.52490234375</v>
+      </c>
+      <c r="H63" t="n">
+        <v>12592.9482421875</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK5_orgE6_ultra</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>50</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E64" t="n">
+        <v>8.48291015625</v>
+      </c>
+      <c r="F64" t="n">
+        <v>7.218611240386963</v>
+      </c>
+      <c r="G64" t="n">
+        <v>4805.20361328125</v>
+      </c>
+      <c r="H64" t="n">
+        <v>10226.740234375</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_ref</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>50</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E65" t="n">
+        <v>9.859785079956055</v>
+      </c>
+      <c r="F65" t="n">
+        <v>8.419105529785156</v>
+      </c>
+      <c r="G65" t="n">
+        <v>5450.4501953125</v>
+      </c>
+      <c r="H65" t="n">
+        <v>10326.5595703125</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK5</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>50</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E66" t="n">
+        <v>9.401267051696777</v>
+      </c>
+      <c r="F66" t="n">
+        <v>8.014777183532715</v>
+      </c>
+      <c r="G66" t="n">
+        <v>5274.75439453125</v>
+      </c>
+      <c r="H66" t="n">
+        <v>10691.224609375</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK20</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>50</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_orgK5</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>50</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_orgK20</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>50</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relE1</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>50</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relE3</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>50</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_orgE1</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>50</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_orgE3</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>50</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E73" t="n">
+        <v>8.656069755554199</v>
+      </c>
+      <c r="F73" t="n">
+        <v>7.39522123336792</v>
+      </c>
+      <c r="G73" t="n">
+        <v>5028.369140625</v>
+      </c>
+      <c r="H73" t="n">
+        <v>10254.7314453125</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK5_orgE1</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>50</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK5_orgE3</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>50</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E75" t="n">
+        <v>8.64002799987793</v>
+      </c>
+      <c r="F75" t="n">
+        <v>7.377531051635742</v>
+      </c>
+      <c r="G75" t="n">
+        <v>5137.50537109375</v>
+      </c>
+      <c r="H75" t="n">
+        <v>10848.1591796875</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>icml_nE_tsp50_relK5_orgE6_ultra</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>50</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E76" t="n">
+        <v>8.475484848022461</v>
+      </c>
+      <c r="F76" t="n">
+        <v>7.216639041900635</v>
+      </c>
+      <c r="G76" t="n">
+        <v>4843.26904296875</v>
+      </c>
+      <c r="H76" t="n">
+        <v>9583.1337890625</v>
+      </c>
+      <c r="I76" t="inlineStr">
         <is>
           <t>F</t>
         </is>

</xml_diff>